<commit_message>
working on excel validation
</commit_message>
<xml_diff>
--- a/capstone/eOPT-Capstone.xlsx
+++ b/capstone/eOPT-Capstone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmlon\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AC63195B-001E-44BE-94E6-715923F0DDB9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FE97678E-9BE1-41CB-8086-D967834D992B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2" xr2:uid="{40B8CE9B-33CA-4882-A633-999552A6A925}"/>
   </bookViews>
@@ -1007,6 +1007,70 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -1061,70 +1125,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -1594,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CC034D-EC3F-4CAC-A6F7-4373A9F5616A}">
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1607,24 +1607,24 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="85" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="85"/>
-      <c r="G1" s="84" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="60"/>
+      <c r="G1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="84"/>
+      <c r="H1" s="59"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="86"/>
+      <c r="K1" s="61"/>
       <c r="L1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1634,26 +1634,26 @@
       </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
-      <c r="Q1" s="87">
-        <v>0</v>
-      </c>
-      <c r="R1" s="87"/>
+      <c r="Q1" s="62">
+        <v>0</v>
+      </c>
+      <c r="R1" s="62"/>
       <c r="S1" s="4"/>
-      <c r="T1" s="88" t="s">
+      <c r="T1" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="88"/>
-      <c r="V1" s="88"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="76" t="s">
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="77">
-        <v>0</v>
-      </c>
-      <c r="AB1" s="77"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="72">
+        <v>0</v>
+      </c>
+      <c r="AB1" s="72"/>
       <c r="AC1" s="5"/>
       <c r="AD1" s="5"/>
       <c r="AE1" s="5"/>
@@ -1662,22 +1662,22 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79" t="s">
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80" t="s">
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="80"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
       <c r="L2" s="6"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4" t="s">
@@ -1685,24 +1685,24 @@
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="82">
-        <v>0</v>
-      </c>
-      <c r="R2" s="82"/>
+      <c r="Q2" s="67">
+        <v>0</v>
+      </c>
+      <c r="R2" s="67"/>
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Y2" s="76" t="s">
+      <c r="Y2" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="76"/>
-      <c r="AA2" s="83">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="83"/>
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="73">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="73"/>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
@@ -1711,110 +1711,110 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="73" t="s">
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="74">
-        <v>0</v>
-      </c>
-      <c r="M3" s="74"/>
-      <c r="N3" s="73" t="s">
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="69">
+        <v>0</v>
+      </c>
+      <c r="M3" s="69"/>
+      <c r="N3" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="74">
-        <v>0</v>
-      </c>
-      <c r="V3" s="74"/>
-      <c r="W3" s="75" t="s">
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="69">
+        <v>0</v>
+      </c>
+      <c r="V3" s="69"/>
+      <c r="W3" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="75"/>
-      <c r="Z3" s="75"/>
-      <c r="AA3" s="75"/>
-      <c r="AB3" s="75"/>
-      <c r="AC3" s="64" t="s">
+      <c r="X3" s="70"/>
+      <c r="Y3" s="70"/>
+      <c r="Z3" s="70"/>
+      <c r="AA3" s="70"/>
+      <c r="AB3" s="70"/>
+      <c r="AC3" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="AD3" s="64"/>
+      <c r="AD3" s="80"/>
       <c r="AE3" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
-      <c r="B4" s="67" t="s">
+      <c r="A4" s="81"/>
+      <c r="B4" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67" t="s">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67" t="s">
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67" t="s">
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="68" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="68"/>
-      <c r="P4" s="68"/>
-      <c r="Q4" s="68" t="s">
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="68"/>
-      <c r="S4" s="68"/>
-      <c r="T4" s="68" t="s">
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="67"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="70" t="s">
+      <c r="U4" s="83"/>
+      <c r="V4" s="85"/>
+      <c r="W4" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="X4" s="71"/>
-      <c r="Y4" s="59" t="s">
+      <c r="X4" s="87"/>
+      <c r="Y4" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="60" t="s">
+      <c r="Z4" s="75"/>
+      <c r="AA4" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="AB4" s="61"/>
-      <c r="AC4" s="62"/>
-      <c r="AD4" s="63" t="s">
+      <c r="AB4" s="77"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="AE4" s="63"/>
+      <c r="AE4" s="79"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
+      <c r="A5" s="82"/>
       <c r="B5" s="10" t="s">
         <v>24</v>
       </c>
@@ -1910,26 +1910,52 @@
       <c r="A6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
+      <c r="B6" s="19">
+        <v>2</v>
+      </c>
+      <c r="C6" s="19">
+        <v>2</v>
+      </c>
       <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="E6" s="19">
+        <v>2</v>
+      </c>
+      <c r="F6" s="19">
+        <v>2</v>
+      </c>
       <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
+      <c r="H6" s="19">
+        <v>2</v>
+      </c>
+      <c r="I6" s="19">
+        <v>2</v>
+      </c>
       <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
+      <c r="K6" s="19">
+        <v>2</v>
+      </c>
+      <c r="L6" s="19">
+        <v>2</v>
+      </c>
       <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="N6" s="19">
+        <v>2</v>
+      </c>
+      <c r="O6" s="19">
+        <v>2</v>
+      </c>
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
+      <c r="R6" s="19">
+        <v>2</v>
+      </c>
       <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
+      <c r="T6" s="19">
+        <v>2</v>
+      </c>
+      <c r="U6" s="19">
+        <v>2</v>
+      </c>
       <c r="V6" s="20"/>
       <c r="W6" s="21">
         <v>0</v>
@@ -1956,25 +1982,51 @@
       <c r="B7" s="19">
         <v>2</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="19">
+        <v>2</v>
+      </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="E7" s="19">
+        <v>2</v>
+      </c>
+      <c r="F7" s="19">
+        <v>2</v>
+      </c>
       <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="19">
+        <v>2</v>
+      </c>
+      <c r="I7" s="19">
+        <v>2</v>
+      </c>
       <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
+      <c r="K7" s="19">
+        <v>2</v>
+      </c>
+      <c r="L7" s="19">
+        <v>2</v>
+      </c>
       <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="N7" s="19">
+        <v>2</v>
+      </c>
+      <c r="O7" s="19">
+        <v>2</v>
+      </c>
       <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
+      <c r="Q7" s="19">
+        <v>2</v>
+      </c>
+      <c r="R7" s="19">
+        <v>2</v>
+      </c>
       <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
+      <c r="T7" s="19">
+        <v>2</v>
+      </c>
+      <c r="U7" s="19">
+        <v>2</v>
+      </c>
       <c r="V7" s="20"/>
       <c r="W7" s="29">
         <v>0</v>
@@ -1998,26 +2050,54 @@
       <c r="A8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
+      <c r="B8" s="19">
+        <v>2</v>
+      </c>
+      <c r="C8" s="19">
+        <v>2</v>
+      </c>
       <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="E8" s="19">
+        <v>2</v>
+      </c>
+      <c r="F8" s="19">
+        <v>2</v>
+      </c>
       <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
+      <c r="H8" s="19">
+        <v>2</v>
+      </c>
+      <c r="I8" s="19">
+        <v>2</v>
+      </c>
       <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+      <c r="K8" s="19">
+        <v>2</v>
+      </c>
+      <c r="L8" s="19">
+        <v>2</v>
+      </c>
       <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="N8" s="19">
+        <v>2</v>
+      </c>
+      <c r="O8" s="19">
+        <v>2</v>
+      </c>
       <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
+      <c r="Q8" s="19">
+        <v>2</v>
+      </c>
+      <c r="R8" s="19">
+        <v>2</v>
+      </c>
       <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
+      <c r="T8" s="19">
+        <v>2</v>
+      </c>
+      <c r="U8" s="19">
+        <v>2</v>
+      </c>
       <c r="V8" s="20"/>
       <c r="W8" s="34">
         <v>0</v>
@@ -2041,26 +2121,54 @@
       <c r="A9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
+      <c r="B9" s="19">
+        <v>2</v>
+      </c>
+      <c r="C9" s="19">
+        <v>2</v>
+      </c>
       <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="E9" s="19">
+        <v>2</v>
+      </c>
+      <c r="F9" s="19">
+        <v>2</v>
+      </c>
       <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="19">
+        <v>2</v>
+      </c>
+      <c r="I9" s="19">
+        <v>2</v>
+      </c>
       <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="K9" s="19">
+        <v>2</v>
+      </c>
+      <c r="L9" s="19">
+        <v>2</v>
+      </c>
       <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
+      <c r="N9" s="19">
+        <v>2</v>
+      </c>
+      <c r="O9" s="19">
+        <v>2</v>
+      </c>
       <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
+      <c r="Q9" s="19">
+        <v>2</v>
+      </c>
+      <c r="R9" s="19">
+        <v>2</v>
+      </c>
       <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
+      <c r="T9" s="19">
+        <v>2</v>
+      </c>
+      <c r="U9" s="19">
+        <v>2</v>
+      </c>
       <c r="V9" s="20"/>
       <c r="W9" s="35">
         <v>0</v>
@@ -2084,26 +2192,54 @@
       <c r="A10" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
+      <c r="B10" s="19">
+        <v>2</v>
+      </c>
+      <c r="C10" s="19">
+        <v>2</v>
+      </c>
       <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="19">
+        <v>2</v>
+      </c>
+      <c r="F10" s="19">
+        <v>2</v>
+      </c>
       <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
+      <c r="H10" s="19">
+        <v>2</v>
+      </c>
+      <c r="I10" s="19">
+        <v>2</v>
+      </c>
       <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
+      <c r="K10" s="19">
+        <v>2</v>
+      </c>
+      <c r="L10" s="19">
+        <v>2</v>
+      </c>
       <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
+      <c r="N10" s="19">
+        <v>2</v>
+      </c>
+      <c r="O10" s="19">
+        <v>2</v>
+      </c>
       <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
+      <c r="Q10" s="19">
+        <v>2</v>
+      </c>
+      <c r="R10" s="19">
+        <v>2</v>
+      </c>
       <c r="S10" s="37"/>
-      <c r="T10" s="37"/>
-      <c r="U10" s="37"/>
+      <c r="T10" s="19">
+        <v>2</v>
+      </c>
+      <c r="U10" s="19">
+        <v>2</v>
+      </c>
       <c r="V10" s="38"/>
       <c r="W10" s="34">
         <v>0</v>
@@ -2127,26 +2263,54 @@
       <c r="A11" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
+      <c r="B11" s="19">
+        <v>2</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2</v>
+      </c>
       <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="19">
+        <v>2</v>
+      </c>
+      <c r="F11" s="19">
+        <v>2</v>
+      </c>
       <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="H11" s="19">
+        <v>2</v>
+      </c>
+      <c r="I11" s="19">
+        <v>2</v>
+      </c>
       <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
+      <c r="K11" s="19">
+        <v>2</v>
+      </c>
+      <c r="L11" s="19">
+        <v>2</v>
+      </c>
       <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
+      <c r="N11" s="19">
+        <v>2</v>
+      </c>
+      <c r="O11" s="19">
+        <v>2</v>
+      </c>
       <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
+      <c r="Q11" s="19">
+        <v>2</v>
+      </c>
+      <c r="R11" s="19">
+        <v>2</v>
+      </c>
       <c r="S11" s="37"/>
-      <c r="T11" s="37"/>
-      <c r="U11" s="37"/>
+      <c r="T11" s="19">
+        <v>2</v>
+      </c>
+      <c r="U11" s="19">
+        <v>2</v>
+      </c>
       <c r="V11" s="38"/>
       <c r="W11" s="42">
         <v>0</v>
@@ -2170,26 +2334,54 @@
       <c r="A12" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
+      <c r="B12" s="19">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19">
+        <v>2</v>
+      </c>
       <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
+      <c r="E12" s="19">
+        <v>2</v>
+      </c>
+      <c r="F12" s="19">
+        <v>2</v>
+      </c>
       <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="H12" s="19">
+        <v>2</v>
+      </c>
+      <c r="I12" s="19">
+        <v>2</v>
+      </c>
       <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
+      <c r="K12" s="19">
+        <v>2</v>
+      </c>
+      <c r="L12" s="19">
+        <v>2</v>
+      </c>
       <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
+      <c r="N12" s="19">
+        <v>2</v>
+      </c>
+      <c r="O12" s="19">
+        <v>2</v>
+      </c>
       <c r="P12" s="37"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
+      <c r="Q12" s="19">
+        <v>2</v>
+      </c>
+      <c r="R12" s="19">
+        <v>2</v>
+      </c>
       <c r="S12" s="37"/>
-      <c r="T12" s="37"/>
-      <c r="U12" s="37"/>
+      <c r="T12" s="19">
+        <v>2</v>
+      </c>
+      <c r="U12" s="19">
+        <v>2</v>
+      </c>
       <c r="V12" s="38"/>
       <c r="W12" s="29">
         <v>0</v>
@@ -2213,26 +2405,54 @@
       <c r="A13" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
+      <c r="B13" s="19">
+        <v>2</v>
+      </c>
+      <c r="C13" s="19">
+        <v>2</v>
+      </c>
       <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="19">
+        <v>2</v>
+      </c>
+      <c r="F13" s="19">
+        <v>2</v>
+      </c>
       <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
+      <c r="H13" s="19">
+        <v>2</v>
+      </c>
+      <c r="I13" s="19">
+        <v>2</v>
+      </c>
       <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
+      <c r="K13" s="19">
+        <v>2</v>
+      </c>
+      <c r="L13" s="19">
+        <v>2</v>
+      </c>
       <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
+      <c r="N13" s="19">
+        <v>2</v>
+      </c>
+      <c r="O13" s="19">
+        <v>2</v>
+      </c>
       <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
+      <c r="Q13" s="19">
+        <v>2</v>
+      </c>
+      <c r="R13" s="19">
+        <v>2</v>
+      </c>
       <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
+      <c r="T13" s="19">
+        <v>2</v>
+      </c>
+      <c r="U13" s="19">
+        <v>2</v>
+      </c>
       <c r="V13" s="38"/>
       <c r="W13" s="35">
         <v>0</v>
@@ -2256,26 +2476,54 @@
       <c r="A14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
+      <c r="B14" s="19">
+        <v>2</v>
+      </c>
+      <c r="C14" s="19">
+        <v>2</v>
+      </c>
       <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="E14" s="19">
+        <v>2</v>
+      </c>
+      <c r="F14" s="19">
+        <v>2</v>
+      </c>
       <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="H14" s="19">
+        <v>2</v>
+      </c>
+      <c r="I14" s="19">
+        <v>2</v>
+      </c>
       <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
+      <c r="K14" s="19">
+        <v>2</v>
+      </c>
+      <c r="L14" s="19">
+        <v>2</v>
+      </c>
       <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
+      <c r="N14" s="19">
+        <v>2</v>
+      </c>
+      <c r="O14" s="19">
+        <v>2</v>
+      </c>
       <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
+      <c r="Q14" s="19">
+        <v>2</v>
+      </c>
+      <c r="R14" s="19">
+        <v>2</v>
+      </c>
       <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
+      <c r="T14" s="19">
+        <v>2</v>
+      </c>
+      <c r="U14" s="19">
+        <v>2</v>
+      </c>
       <c r="V14" s="20"/>
       <c r="W14" s="35">
         <v>0</v>
@@ -2309,26 +2557,54 @@
       <c r="A15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="19">
+        <v>2</v>
+      </c>
+      <c r="C15" s="19">
+        <v>2</v>
+      </c>
       <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="E15" s="19">
+        <v>2</v>
+      </c>
+      <c r="F15" s="19">
+        <v>2</v>
+      </c>
       <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="H15" s="19">
+        <v>2</v>
+      </c>
+      <c r="I15" s="19">
+        <v>2</v>
+      </c>
       <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
+      <c r="K15" s="19">
+        <v>2</v>
+      </c>
+      <c r="L15" s="19">
+        <v>2</v>
+      </c>
       <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
+      <c r="N15" s="19">
+        <v>2</v>
+      </c>
+      <c r="O15" s="19">
+        <v>2</v>
+      </c>
       <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
+      <c r="Q15" s="19">
+        <v>2</v>
+      </c>
+      <c r="R15" s="19">
+        <v>2</v>
+      </c>
       <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
+      <c r="T15" s="19">
+        <v>2</v>
+      </c>
+      <c r="U15" s="19">
+        <v>2</v>
+      </c>
       <c r="V15" s="20"/>
       <c r="W15" s="35">
         <v>0</v>
@@ -2362,26 +2638,54 @@
       <c r="A16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="19">
+        <v>2</v>
+      </c>
+      <c r="C16" s="19">
+        <v>2</v>
+      </c>
       <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="E16" s="19">
+        <v>2</v>
+      </c>
+      <c r="F16" s="19">
+        <v>2</v>
+      </c>
       <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="H16" s="19">
+        <v>2</v>
+      </c>
+      <c r="I16" s="19">
+        <v>2</v>
+      </c>
       <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
+      <c r="K16" s="19">
+        <v>2</v>
+      </c>
+      <c r="L16" s="19">
+        <v>2</v>
+      </c>
       <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
+      <c r="N16" s="19">
+        <v>2</v>
+      </c>
+      <c r="O16" s="19">
+        <v>2</v>
+      </c>
       <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
+      <c r="Q16" s="19">
+        <v>2</v>
+      </c>
+      <c r="R16" s="19">
+        <v>2</v>
+      </c>
       <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="19"/>
+      <c r="T16" s="19">
+        <v>2</v>
+      </c>
+      <c r="U16" s="19">
+        <v>2</v>
+      </c>
       <c r="V16" s="20"/>
       <c r="W16" s="35">
         <v>0</v>
@@ -2415,26 +2719,54 @@
       <c r="A17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="19">
+        <v>2</v>
+      </c>
+      <c r="C17" s="19">
+        <v>2</v>
+      </c>
       <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="E17" s="19">
+        <v>2</v>
+      </c>
+      <c r="F17" s="19">
+        <v>2</v>
+      </c>
       <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="H17" s="19">
+        <v>2</v>
+      </c>
+      <c r="I17" s="19">
+        <v>2</v>
+      </c>
       <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+      <c r="K17" s="19">
+        <v>2</v>
+      </c>
+      <c r="L17" s="19">
+        <v>2</v>
+      </c>
       <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
+      <c r="N17" s="19">
+        <v>2</v>
+      </c>
+      <c r="O17" s="19">
+        <v>2</v>
+      </c>
       <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
+      <c r="Q17" s="19">
+        <v>2</v>
+      </c>
+      <c r="R17" s="19">
+        <v>2</v>
+      </c>
       <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
+      <c r="T17" s="19">
+        <v>2</v>
+      </c>
+      <c r="U17" s="19">
+        <v>2</v>
+      </c>
       <c r="V17" s="20"/>
       <c r="W17" s="35">
         <v>0</v>
@@ -2468,26 +2800,54 @@
       <c r="A18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
+      <c r="B18" s="19">
+        <v>2</v>
+      </c>
+      <c r="C18" s="19">
+        <v>2</v>
+      </c>
       <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="E18" s="19">
+        <v>2</v>
+      </c>
+      <c r="F18" s="19">
+        <v>2</v>
+      </c>
       <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
+      <c r="H18" s="19">
+        <v>2</v>
+      </c>
+      <c r="I18" s="19">
+        <v>2</v>
+      </c>
       <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
+      <c r="K18" s="19">
+        <v>2</v>
+      </c>
+      <c r="L18" s="19">
+        <v>2</v>
+      </c>
       <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
+      <c r="N18" s="19">
+        <v>2</v>
+      </c>
+      <c r="O18" s="19">
+        <v>2</v>
+      </c>
       <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
+      <c r="Q18" s="19">
+        <v>2</v>
+      </c>
+      <c r="R18" s="19">
+        <v>2</v>
+      </c>
       <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
+      <c r="T18" s="19">
+        <v>2</v>
+      </c>
+      <c r="U18" s="19">
+        <v>2</v>
+      </c>
       <c r="V18" s="20"/>
       <c r="W18" s="35">
         <v>0</v>
@@ -2519,24 +2879,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="N3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:AB3"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="T1:X1"/>
     <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AD4:AE4"/>
@@ -2553,6 +2895,24 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:K3"/>
     <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:AB3"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <conditionalFormatting sqref="AE3">
     <cfRule type="containsBlanks" dxfId="10" priority="10">

</xml_diff>